<commit_message>
Fix test_convergence latex generation (infty norm). Also fix serialization methods which use datetime to generate a unique directory name. Add a 1.1 sec delay so that multiple calls very quickly do not overlap in output dir. A little stupid, but ...
</commit_message>
<xml_diff>
--- a/convergence_test2.xlsx
+++ b/convergence_test2.xlsx
@@ -498,7 +498,7 @@
         <v>32</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -533,22 +533,22 @@
         <v>28</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003220637498853707</v>
+        <v>0.003528628827193514</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005200615837365613</v>
+        <v>0.005619520991774325</v>
       </c>
       <c r="F3" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G3" t="n">
-        <v>0.008966949877949659</v>
+        <v>0.01043734166128485</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00764563067704227</v>
+        <v>0.008195667896686389</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -568,22 +568,22 @@
         <v>24</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007140773762873864</v>
+        <v>0.007946586843113446</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01153076716503</v>
+        <v>0.0126553439777203</v>
       </c>
       <c r="F4" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G4" t="n">
-        <v>0.02013973478694431</v>
+        <v>0.02353525321227257</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01717205696590392</v>
+        <v>0.01848048338857031</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -603,22 +603,22 @@
         <v>20</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01461410628266141</v>
+        <v>0.01606891090935042</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02359854302435592</v>
+        <v>0.02559055842715701</v>
       </c>
       <c r="F5" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G5" t="n">
-        <v>0.04227137577197215</v>
+        <v>0.04887858320107918</v>
       </c>
       <c r="H5" t="n">
-        <v>0.03604250405789834</v>
+        <v>0.03838071495374291</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -638,22 +638,22 @@
         <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02505435434594949</v>
+        <v>0.02754260422669819</v>
       </c>
       <c r="E6" t="n">
-        <v>0.04045722999030184</v>
+        <v>0.04386299897208617</v>
       </c>
       <c r="F6" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G6" t="n">
-        <v>0.07129250894470629</v>
+        <v>0.08242379185190507</v>
       </c>
       <c r="H6" t="n">
-        <v>0.06078724659444527</v>
+        <v>0.06472127163466472</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -673,22 +673,22 @@
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D7" t="n">
-        <v>0.03618104369111369</v>
+        <v>0.04003080472359422</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05842436750469263</v>
+        <v>0.06375109383232384</v>
       </c>
       <c r="F7" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G7" t="n">
-        <v>0.09853950610589757</v>
+        <v>0.1143468201407329</v>
       </c>
       <c r="H7" t="n">
-        <v>0.08401927980399425</v>
+        <v>0.08978805076313018</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -708,22 +708,22 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06707980191457164</v>
+        <v>0.07342140686978549</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1083190145828069</v>
+        <v>0.1169273271166121</v>
       </c>
       <c r="F8" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1783136275537619</v>
+        <v>0.2044475054171753</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1520383362811282</v>
+        <v>0.1605374156640277</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -743,22 +743,22 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6192800236683373</v>
+        <v>0.6279234177358902</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1597345059143589</v>
+        <v>0.1726146320864818</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2579358283966005</v>
+        <v>0.2748975865701587</v>
       </c>
       <c r="F9" t="n">
-        <v>1.172820170986672</v>
+        <v>1.27351935105921</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3849089900690978</v>
+        <v>0.4331075750530472</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3281909704411726</v>
+        <v>0.3400871566598682</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>

</xml_diff>